<commit_message>
newer version of product list
</commit_message>
<xml_diff>
--- a/config/out_of_stock.xlsx
+++ b/config/out_of_stock.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15" conformance="strict">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr dateCompatibility="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\APanov\why_sales_going_down\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\APanov\why_sales_going_down\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,11 +18,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Out-of-Stock Master list'!$A$1:$K$807</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4821" uniqueCount="1675">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="4821" uniqueCount="1675">
   <si>
     <t>Retailer</t>
   </si>
@@ -5052,7 +5057,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5380,15 +5385,15 @@
   </fills>
   <borders count="10">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="thick">
         <color theme="4"/>
@@ -5396,8 +5401,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="thick">
         <color theme="4" tint="0.499984740745262"/>
@@ -5405,8 +5410,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.39997558519241921"/>
@@ -5414,12 +5419,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <start style="thin">
         <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
+      </start>
+      <end style="thin">
         <color rgb="FF7F7F7F"/>
-      </right>
+      </end>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
       </top>
@@ -5429,12 +5434,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <start style="thin">
         <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
+      </start>
+      <end style="thin">
         <color rgb="FF3F3F3F"/>
-      </right>
+      </end>
       <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -5444,8 +5449,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -5453,12 +5458,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <start style="double">
         <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
+      </start>
+      <end style="double">
         <color rgb="FF3F3F3F"/>
-      </right>
+      </end>
       <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -5468,12 +5473,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <start style="thin">
         <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
+      </start>
+      <end style="thin">
         <color rgb="FFB2B2B2"/>
-      </right>
+      </end>
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
@@ -5483,8 +5488,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -5618,7 +5623,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5737,25 +5742,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:lumMod val="110%"/>
+                <a:satMod val="105%"/>
+                <a:tint val="67%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="103%"/>
+                <a:tint val="73%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="109%"/>
+                <a:tint val="81%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -5763,25 +5768,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:satMod val="103%"/>
+                <a:lumMod val="102%"/>
+                <a:tint val="94%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:satMod val="110%"/>
+                <a:lumMod val="100%"/>
+                <a:shade val="100%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:lumMod val="99%"/>
+                <a:satMod val="120%"/>
+                <a:shade val="78%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -5794,21 +5799,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -5822,7 +5827,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="63%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -5834,32 +5839,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
+            <a:tint val="95%"/>
+            <a:satMod val="170%"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="93%"/>
+                <a:satMod val="150%"/>
+                <a:shade val="98%"/>
+                <a:lumMod val="102%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="98%"/>
+                <a:satMod val="130%"/>
+                <a:shade val="90%"/>
+                <a:lumMod val="103%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="63%"/>
+                <a:satMod val="120%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -5879,12 +5884,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K807"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23269,7 +23274,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A63631C-0DCB-42A1-AC1D-BCAA6B2D4125}">
+<ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{5A63631C-0DCB-42A1-AC1D-BCAA6B2D4125}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/SolverFoundationForExcel/Version"/>
   </ds:schemaRefs>

</xml_diff>

<commit_message>
the last version of the product list
</commit_message>
<xml_diff>
--- a/config/out_of_stock.xlsx
+++ b/config/out_of_stock.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4495" uniqueCount="1552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4495" uniqueCount="1553">
   <si>
     <t>Retailer</t>
   </si>
@@ -4678,6 +4678,9 @@
   </si>
   <si>
     <t>http://m.saks.com/pd.jsp?productCode=0400088522630</t>
+  </si>
+  <si>
+    <t>Eau de Parfum</t>
   </si>
 </sst>
 </file>
@@ -5527,9 +5530,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K733"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A697" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K704" sqref="K704"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20403,7 +20406,7 @@
         <v>1483</v>
       </c>
       <c r="K704" t="s">
-        <v>15</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="705" spans="1:11" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed the expected title
</commit_message>
<xml_diff>
--- a/config/out_of_stock.xlsx
+++ b/config/out_of_stock.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3779" uniqueCount="1291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3780" uniqueCount="1291">
   <si>
     <t>Retailer</t>
   </si>
@@ -4791,9 +4791,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K643"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K88" sqref="K88"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A607" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C610" sqref="C610"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17770,9 +17770,8 @@
       <c r="J611" s="8" t="s">
         <v>1236</v>
       </c>
-      <c r="K611" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>Wonderlust Sensual Essense</v>
+      <c r="K611" s="19" t="s">
+        <v>1264</v>
       </c>
     </row>
     <row r="612" spans="1:11" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed the retailer name
</commit_message>
<xml_diff>
--- a/config/out_of_stock.xlsx
+++ b/config/out_of_stock.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3780" uniqueCount="1291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3780" uniqueCount="1290">
   <si>
     <t>Retailer</t>
   </si>
@@ -3745,9 +3745,6 @@
   </si>
   <si>
     <t>http://www.thebay.com/webapp/wcs/stores/servlet/en/thebay/beauty/fragrance/sexy-ruby-eau-de-parfum-50ml-0600089457750--24</t>
-  </si>
-  <si>
-    <t>Stage</t>
   </si>
   <si>
     <t>1oz, 1.7oz, 3.4oz</t>
@@ -4791,9 +4788,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K643"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A607" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C610" sqref="C610"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6650,7 +6647,7 @@
         <v>148</v>
       </c>
       <c r="K85" s="21" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -6671,7 +6668,7 @@
         <v>149</v>
       </c>
       <c r="K86" s="21" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -6695,7 +6692,7 @@
         <v>150</v>
       </c>
       <c r="K87" s="21" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -13703,7 +13700,7 @@
         <v>30</v>
       </c>
       <c r="J419" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="K419" s="4" t="s">
         <v>10</v>
@@ -15184,7 +15181,7 @@
         <v>30</v>
       </c>
       <c r="J490" s="8" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="K490" s="4" t="s">
         <v>10</v>
@@ -15500,7 +15497,7 @@
         <v>1067</v>
       </c>
       <c r="J503" s="20" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="K503" s="4" t="s">
         <v>1066</v>
@@ -15541,7 +15538,7 @@
         <v>1070</v>
       </c>
       <c r="J505" s="20" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="K505" s="4" t="str">
         <f t="shared" si="0"/>
@@ -15562,7 +15559,7 @@
         <v>1072</v>
       </c>
       <c r="J506" s="20" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="K506" s="4" t="str">
         <f t="shared" si="0"/>
@@ -15583,7 +15580,7 @@
         <v>1073</v>
       </c>
       <c r="J507" s="20" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="K507" s="4" t="str">
         <f t="shared" si="0"/>
@@ -15625,7 +15622,7 @@
         <v>1076</v>
       </c>
       <c r="J509" s="20" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="K509" s="4" t="str">
         <f t="shared" si="0"/>
@@ -16123,7 +16120,7 @@
         <v>15</v>
       </c>
       <c r="C533" s="17" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="D533" s="14" t="s">
         <v>1095</v>
@@ -16133,7 +16130,7 @@
         <v>1114</v>
       </c>
       <c r="K533" s="17" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="534" spans="1:11" x14ac:dyDescent="0.25">
@@ -17708,7 +17705,7 @@
         <v>1232</v>
       </c>
       <c r="K608" s="18" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="609" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -17740,7 +17737,7 @@
         <v>15</v>
       </c>
       <c r="C610" s="17" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="D610" s="14" t="s">
         <v>1070</v>
@@ -17771,7 +17768,7 @@
         <v>1236</v>
       </c>
       <c r="K611" s="19" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="612" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -17860,7 +17857,7 @@
     </row>
     <row r="616" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A616" s="5" t="s">
-        <v>1241</v>
+        <v>1032</v>
       </c>
       <c r="B616" s="4" t="s">
         <v>15</v>
@@ -17869,10 +17866,10 @@
         <v>1066</v>
       </c>
       <c r="D616" s="5" t="s">
+        <v>1241</v>
+      </c>
+      <c r="J616" s="8" t="s">
         <v>1242</v>
-      </c>
-      <c r="J616" s="8" t="s">
-        <v>1243</v>
       </c>
       <c r="K616" s="4" t="str">
         <f t="shared" si="4"/>
@@ -17881,7 +17878,7 @@
     </row>
     <row r="617" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A617" s="5" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B617" s="4" t="s">
         <v>15</v>
@@ -17893,7 +17890,7 @@
         <v>1070</v>
       </c>
       <c r="J617" s="8" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="K617" s="5" t="str">
         <f t="shared" si="4"/>
@@ -17902,7 +17899,7 @@
     </row>
     <row r="618" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A618" s="5" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B618" s="4" t="s">
         <v>21</v>
@@ -17914,7 +17911,7 @@
         <v>1070</v>
       </c>
       <c r="J618" s="8" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="K618" s="4" t="str">
         <f t="shared" si="4"/>
@@ -17923,7 +17920,7 @@
     </row>
     <row r="619" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A619" s="5" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B619" s="4" t="s">
         <v>15</v>
@@ -17935,7 +17932,7 @@
         <v>1070</v>
       </c>
       <c r="J619" s="8" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="K619" s="4" t="str">
         <f t="shared" si="4"/>
@@ -17944,7 +17941,7 @@
     </row>
     <row r="620" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A620" s="5" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B620" s="4" t="s">
         <v>15</v>
@@ -17956,7 +17953,7 @@
         <v>1067</v>
       </c>
       <c r="J620" s="8" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="K620" s="4" t="str">
         <f t="shared" si="4"/>
@@ -17965,7 +17962,7 @@
     </row>
     <row r="621" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A621" s="5" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B621" s="4" t="s">
         <v>21</v>
@@ -17977,7 +17974,7 @@
         <v>1067</v>
       </c>
       <c r="J621" s="8" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="K621" s="4" t="str">
         <f t="shared" si="4"/>
@@ -17986,7 +17983,7 @@
     </row>
     <row r="622" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A622" s="5" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B622" s="4" t="s">
         <v>15</v>
@@ -17998,7 +17995,7 @@
         <v>1067</v>
       </c>
       <c r="J622" s="8" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="K622" s="5" t="str">
         <f t="shared" si="4"/>
@@ -18007,7 +18004,7 @@
     </row>
     <row r="623" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A623" s="5" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B623" s="4" t="s">
         <v>9</v>
@@ -18019,7 +18016,7 @@
         <v>1067</v>
       </c>
       <c r="J623" s="8" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="K623" s="4" t="str">
         <f t="shared" si="4"/>
@@ -18028,7 +18025,7 @@
     </row>
     <row r="624" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A624" s="5" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B624" s="4" t="s">
         <v>15</v>
@@ -18040,7 +18037,7 @@
         <v>1214</v>
       </c>
       <c r="J624" s="8" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="K624" s="4" t="str">
         <f t="shared" si="4"/>
@@ -18049,7 +18046,7 @@
     </row>
     <row r="625" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A625" s="5" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B625" s="4" t="s">
         <v>15</v>
@@ -18061,7 +18058,7 @@
         <v>1214</v>
       </c>
       <c r="J625" s="8" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="K625" s="5" t="str">
         <f t="shared" si="4"/>
@@ -18070,7 +18067,7 @@
     </row>
     <row r="626" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A626" s="5" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B626" s="4" t="s">
         <v>15</v>
@@ -18082,7 +18079,7 @@
         <v>1068</v>
       </c>
       <c r="J626" s="8" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="K626" s="4" t="str">
         <f t="shared" si="4"/>
@@ -18103,7 +18100,7 @@
         <v>1132</v>
       </c>
       <c r="J627" s="8" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="K627" s="4" t="str">
         <f t="shared" si="4"/>
@@ -18121,10 +18118,10 @@
         <v>247</v>
       </c>
       <c r="D628" s="5" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="J628" s="8" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="K628" s="4" t="str">
         <f t="shared" si="4"/>
@@ -18145,7 +18142,7 @@
         <v>1068</v>
       </c>
       <c r="J629" s="8" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="K629" s="4" t="str">
         <f t="shared" si="4"/>
@@ -18166,7 +18163,7 @@
         <v>1070</v>
       </c>
       <c r="J630" s="8" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="K630" s="4" t="str">
         <f t="shared" si="4"/>
@@ -18187,7 +18184,7 @@
         <v>1067</v>
       </c>
       <c r="J631" s="8" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="K631" s="4" t="str">
         <f t="shared" si="4"/>
@@ -18208,7 +18205,7 @@
         <v>1070</v>
       </c>
       <c r="J632" s="8" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="K632" s="5" t="str">
         <f t="shared" si="4"/>
@@ -18229,7 +18226,7 @@
         <v>1070</v>
       </c>
       <c r="J633" s="8" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="K633" s="4" t="str">
         <f t="shared" si="4"/>
@@ -18253,7 +18250,7 @@
         <v>5038303</v>
       </c>
       <c r="J634" s="20" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="K634" s="21" t="str">
         <f t="shared" si="4"/>
@@ -18271,13 +18268,13 @@
         <v>10</v>
       </c>
       <c r="D635" s="19" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="E635" s="7">
         <v>2903322</v>
       </c>
       <c r="J635" s="20" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="K635" s="21" t="str">
         <f t="shared" si="4"/>
@@ -18295,13 +18292,13 @@
         <v>10</v>
       </c>
       <c r="D636" s="19" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="E636" s="7">
         <v>2903321</v>
       </c>
       <c r="J636" s="20" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="K636" s="21" t="str">
         <f t="shared" si="4"/>
@@ -18319,13 +18316,13 @@
         <v>101</v>
       </c>
       <c r="D637" s="19" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="E637" s="7">
         <v>4477346</v>
       </c>
       <c r="J637" s="20" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="K637" s="21" t="str">
         <f t="shared" si="4"/>
@@ -18343,13 +18340,13 @@
         <v>15</v>
       </c>
       <c r="D638" s="19" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E638" s="7">
         <v>5022078</v>
       </c>
       <c r="J638" s="20" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K638" s="21" t="str">
         <f t="shared" si="4"/>
@@ -18364,16 +18361,16 @@
         <v>15</v>
       </c>
       <c r="C639" s="19" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="D639" s="19" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="E639" s="7">
         <v>5273948</v>
       </c>
       <c r="J639" s="20" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="K639" s="21"/>
     </row>
@@ -18394,7 +18391,7 @@
         <v>4963893</v>
       </c>
       <c r="J640" s="20" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="K640" s="21" t="str">
         <f t="shared" si="4"/>
@@ -18418,7 +18415,7 @@
         <v>5302903</v>
       </c>
       <c r="J641" s="20" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="K641" s="19" t="str">
         <f t="shared" si="4"/>
@@ -18433,7 +18430,7 @@
         <v>15</v>
       </c>
       <c r="C642" s="19" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="D642" s="19" t="s">
         <v>1160</v>
@@ -18442,7 +18439,7 @@
         <v>3055885</v>
       </c>
       <c r="J642" s="20" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K642" s="21" t="str">
         <f t="shared" si="4"/>
@@ -18460,13 +18457,13 @@
         <v>1139</v>
       </c>
       <c r="D643" s="19" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="E643" s="7">
         <v>4974682</v>
       </c>
       <c r="J643" s="20" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="K643" s="21" t="str">
         <f t="shared" si="4"/>
@@ -18474,7 +18471,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K643" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K643" xr:uid="{2037A1FD-0D19-4DAD-BF73-9AD404BA20F0}"/>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1" display="https://www.macys.com/shop/product/donna-karan-cashmere-mist-eau-de-parfum-1.7-oz?ID=174838" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="J4" r:id="rId2" display="https://www.macys.com/shop/product/donna-karan-cashmere-mist-eau-de-parfum-spray-3.4-oz?ID=166324" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>